<commit_message>
Add PivotTable in Excel COM; add Query in Access COM
</commit_message>
<xml_diff>
--- a/PowerShell/Outputs/PS_MSO_Spreadsheet.xlsx
+++ b/PowerShell/Outputs/PS_MSO_Spreadsheet.xlsx
@@ -8,14 +8,18 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="https://d.docs.live.net/103b4026c7a1d890/Documents/Databases/COM_Interface/PowerShell/Outputs/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="8_{484D0796-C71E-4B64-93A1-60382BFD63F0}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="8_{5DFFCECB-ABCB-4764-8487-560378F296D8}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="1884" yWindow="828" windowWidth="17280" windowHeight="8964" xr2:uid="{A1AD83EB-E87D-4DA7-8BB2-C2356B00CEC3}"/>
+    <workbookView xWindow="2688" yWindow="2688" windowWidth="17280" windowHeight="8964" activeTab="1" xr2:uid="{27ADC896-2A9D-44D5-8A74-7B25018FBE51}"/>
   </bookViews>
   <sheets>
     <sheet name="METALS" sheetId="1" r:id="rId1"/>
+    <sheet name="PIVOT" sheetId="2" r:id="rId2"/>
   </sheets>
   <calcPr calcId="181029"/>
+  <pivotCaches>
+    <pivotCache cacheId="2" r:id="rId3"/>
+  </pivotCaches>
   <extLst>
     <ext xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" uri="{140A7094-0E35-4892-8432-C4D2E57EDEB5}">
       <x15:workbookPr chartTrackingRefBase="1"/>
@@ -33,7 +37,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="215" uniqueCount="7">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="226" uniqueCount="14">
   <si>
     <t>year</t>
   </si>
@@ -55,11 +59,35 @@
   <si>
     <t>silver</t>
   </si>
+  <si>
+    <t>Row Labels</t>
+  </si>
+  <si>
+    <t>Grand Total</t>
+  </si>
+  <si>
+    <t>Min Price</t>
+  </si>
+  <si>
+    <t>Values</t>
+  </si>
+  <si>
+    <t>Avg Price</t>
+  </si>
+  <si>
+    <t>Max Price</t>
+  </si>
+  <si>
+    <t>Std Price</t>
+  </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
+  <numFmts count="1">
+    <numFmt numFmtId="164" formatCode="&quot;$&quot;#,##0.00"/>
+  </numFmts>
   <fonts count="2" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
@@ -95,14 +123,217 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="2">
+  <cellXfs count="6">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1"/>
+    <xf numFmtId="164" fontId="1" fillId="0" borderId="0" xfId="0" pivotButton="1" applyNumberFormat="1" applyFont="1" applyAlignment="1">
+      <alignment horizontal="right"/>
+    </xf>
+    <xf numFmtId="164" fontId="1" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyAlignment="1">
+      <alignment horizontal="right"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" pivotButton="1" applyFont="1"/>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+      <alignment horizontal="left"/>
+    </xf>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
   </cellStyles>
-  <dxfs count="0"/>
+  <dxfs count="43">
+    <dxf>
+      <font>
+        <color rgb="FF000000"/>
+      </font>
+    </dxf>
+    <dxf>
+      <font>
+        <color rgb="FF000000"/>
+      </font>
+    </dxf>
+    <dxf>
+      <font>
+        <color rgb="FF000000"/>
+      </font>
+    </dxf>
+    <dxf>
+      <font>
+        <color rgb="FF000000"/>
+      </font>
+    </dxf>
+    <dxf>
+      <font>
+        <color rgb="FF000000"/>
+      </font>
+    </dxf>
+    <dxf>
+      <font>
+        <color rgb="FF000000"/>
+      </font>
+    </dxf>
+    <dxf>
+      <font>
+        <color rgb="FF000000"/>
+      </font>
+    </dxf>
+    <dxf>
+      <font>
+        <color rgb="FF000000"/>
+      </font>
+    </dxf>
+    <dxf>
+      <font>
+        <color rgb="FF000000"/>
+      </font>
+    </dxf>
+    <dxf>
+      <font>
+        <sz val="10"/>
+      </font>
+    </dxf>
+    <dxf>
+      <font>
+        <sz val="10"/>
+      </font>
+    </dxf>
+    <dxf>
+      <font>
+        <sz val="10"/>
+      </font>
+    </dxf>
+    <dxf>
+      <font>
+        <sz val="10"/>
+      </font>
+    </dxf>
+    <dxf>
+      <font>
+        <sz val="10"/>
+      </font>
+    </dxf>
+    <dxf>
+      <font>
+        <sz val="10"/>
+      </font>
+    </dxf>
+    <dxf>
+      <font>
+        <sz val="10"/>
+      </font>
+    </dxf>
+    <dxf>
+      <font>
+        <sz val="10"/>
+      </font>
+    </dxf>
+    <dxf>
+      <font>
+        <sz val="10"/>
+      </font>
+    </dxf>
+    <dxf>
+      <font>
+        <name val="Arial"/>
+        <scheme val="none"/>
+      </font>
+    </dxf>
+    <dxf>
+      <font>
+        <name val="Arial"/>
+        <scheme val="none"/>
+      </font>
+    </dxf>
+    <dxf>
+      <font>
+        <name val="Arial"/>
+        <scheme val="none"/>
+      </font>
+    </dxf>
+    <dxf>
+      <font>
+        <name val="Arial"/>
+        <scheme val="none"/>
+      </font>
+    </dxf>
+    <dxf>
+      <font>
+        <name val="Arial"/>
+        <scheme val="none"/>
+      </font>
+    </dxf>
+    <dxf>
+      <font>
+        <name val="Arial"/>
+        <scheme val="none"/>
+      </font>
+    </dxf>
+    <dxf>
+      <font>
+        <name val="Arial"/>
+        <scheme val="none"/>
+      </font>
+    </dxf>
+    <dxf>
+      <font>
+        <name val="Arial"/>
+        <scheme val="none"/>
+      </font>
+    </dxf>
+    <dxf>
+      <font>
+        <name val="Arial"/>
+        <scheme val="none"/>
+      </font>
+    </dxf>
+    <dxf>
+      <alignment horizontal="right"/>
+    </dxf>
+    <dxf>
+      <numFmt numFmtId="164" formatCode="&quot;$&quot;#,##0.00"/>
+    </dxf>
+    <dxf>
+      <alignment horizontal="right"/>
+    </dxf>
+    <dxf>
+      <numFmt numFmtId="164" formatCode="&quot;$&quot;#,##0.00"/>
+    </dxf>
+    <dxf>
+      <alignment horizontal="right"/>
+    </dxf>
+    <dxf>
+      <alignment horizontal="right"/>
+    </dxf>
+    <dxf>
+      <alignment horizontal="right"/>
+    </dxf>
+    <dxf>
+      <numFmt numFmtId="164" formatCode="&quot;$&quot;#,##0.00"/>
+    </dxf>
+    <dxf>
+      <numFmt numFmtId="164" formatCode="&quot;$&quot;#,##0.00"/>
+    </dxf>
+    <dxf>
+      <numFmt numFmtId="164" formatCode="&quot;$&quot;#,##0.00"/>
+    </dxf>
+    <dxf>
+      <alignment horizontal="right"/>
+    </dxf>
+    <dxf>
+      <alignment horizontal="right"/>
+    </dxf>
+    <dxf>
+      <alignment horizontal="right"/>
+    </dxf>
+    <dxf>
+      <numFmt numFmtId="164" formatCode="&quot;$&quot;#,##0.00"/>
+    </dxf>
+    <dxf>
+      <numFmt numFmtId="164" formatCode="&quot;$&quot;#,##0.00"/>
+    </dxf>
+    <dxf>
+      <numFmt numFmtId="164" formatCode="&quot;$&quot;#,##0.00"/>
+    </dxf>
+  </dxfs>
   <tableStyles count="0" defaultTableStyle="TableStyleMedium2" defaultPivotStyle="PivotStyleLight16"/>
   <extLst>
     <ext xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" uri="{EB79DEF2-80B8-43e5-95BD-54CBDDF9020C}">
@@ -113,6 +344,1410 @@
     </ext>
   </extLst>
 </styleSheet>
+</file>
+
+<file path=xl/pivotCache/pivotCacheDefinition1.xml><?xml version="1.0" encoding="utf-8"?>
+<pivotCacheDefinition xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="xr" r:id="rId1" refreshedBy="Parfait Gasana" refreshedDate="44829.639638194443" createdVersion="3" refreshedVersion="8" minRefreshableVersion="3" recordCount="212" xr:uid="{933E7690-CEC4-482E-83A9-D7B4F69EC1D6}">
+  <cacheSource type="worksheet">
+    <worksheetSource ref="A1:C213" sheet="METALS"/>
+  </cacheSource>
+  <cacheFields count="3">
+    <cacheField name="year" numFmtId="0">
+      <sharedItems containsSemiMixedTypes="0" containsString="0" containsNumber="1" containsInteger="1" minValue="1968" maxValue="2020"/>
+    </cacheField>
+    <cacheField name="metal" numFmtId="0">
+      <sharedItems count="4">
+        <s v="gold"/>
+        <s v="palladium"/>
+        <s v="platinum"/>
+        <s v="silver"/>
+      </sharedItems>
+    </cacheField>
+    <cacheField name="avg_price" numFmtId="0">
+      <sharedItems containsString="0" containsBlank="1" containsNumber="1" minValue="1.53633333333333" maxValue="2212.125"/>
+    </cacheField>
+  </cacheFields>
+  <extLst>
+    <ext xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" uri="{725AE2AE-9491-48be-B2B4-4EB974FC3084}">
+      <x14:pivotCacheDefinition/>
+    </ext>
+  </extLst>
+</pivotCacheDefinition>
+</file>
+
+<file path=xl/pivotCache/pivotCacheRecords1.xml><?xml version="1.0" encoding="utf-8"?>
+<pivotCacheRecords xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="xr" count="212">
+  <r>
+    <n v="1968"/>
+    <x v="0"/>
+    <n v="39.822842105263199"/>
+  </r>
+  <r>
+    <n v="1968"/>
+    <x v="1"/>
+    <m/>
+  </r>
+  <r>
+    <n v="1968"/>
+    <x v="2"/>
+    <m/>
+  </r>
+  <r>
+    <n v="1968"/>
+    <x v="3"/>
+    <n v="2.1891673306772899"/>
+  </r>
+  <r>
+    <n v="1969"/>
+    <x v="0"/>
+    <n v="41.112648221343903"/>
+  </r>
+  <r>
+    <n v="1969"/>
+    <x v="1"/>
+    <m/>
+  </r>
+  <r>
+    <n v="1969"/>
+    <x v="2"/>
+    <m/>
+  </r>
+  <r>
+    <n v="1969"/>
+    <x v="3"/>
+    <n v="1.79966535433071"/>
+  </r>
+  <r>
+    <n v="1970"/>
+    <x v="0"/>
+    <n v="35.950236220472398"/>
+  </r>
+  <r>
+    <n v="1970"/>
+    <x v="1"/>
+    <m/>
+  </r>
+  <r>
+    <n v="1970"/>
+    <x v="2"/>
+    <m/>
+  </r>
+  <r>
+    <n v="1970"/>
+    <x v="3"/>
+    <n v="1.76574901960784"/>
+  </r>
+  <r>
+    <n v="1971"/>
+    <x v="0"/>
+    <n v="40.821264822134403"/>
+  </r>
+  <r>
+    <n v="1971"/>
+    <x v="1"/>
+    <m/>
+  </r>
+  <r>
+    <n v="1971"/>
+    <x v="2"/>
+    <m/>
+  </r>
+  <r>
+    <n v="1971"/>
+    <x v="3"/>
+    <n v="1.53633333333333"/>
+  </r>
+  <r>
+    <n v="1972"/>
+    <x v="0"/>
+    <n v="58.230590551181102"/>
+  </r>
+  <r>
+    <n v="1972"/>
+    <x v="1"/>
+    <m/>
+  </r>
+  <r>
+    <n v="1972"/>
+    <x v="2"/>
+    <m/>
+  </r>
+  <r>
+    <n v="1972"/>
+    <x v="3"/>
+    <n v="1.6768968253968299"/>
+  </r>
+  <r>
+    <n v="1973"/>
+    <x v="0"/>
+    <n v="97.315731225296403"/>
+  </r>
+  <r>
+    <n v="1973"/>
+    <x v="1"/>
+    <m/>
+  </r>
+  <r>
+    <n v="1973"/>
+    <x v="2"/>
+    <m/>
+  </r>
+  <r>
+    <n v="1973"/>
+    <x v="3"/>
+    <n v="2.54571020408163"/>
+  </r>
+  <r>
+    <n v="1974"/>
+    <x v="0"/>
+    <n v="158.84604743083"/>
+  </r>
+  <r>
+    <n v="1974"/>
+    <x v="1"/>
+    <m/>
+  </r>
+  <r>
+    <n v="1974"/>
+    <x v="2"/>
+    <m/>
+  </r>
+  <r>
+    <n v="1974"/>
+    <x v="3"/>
+    <n v="4.6715078740157496"/>
+  </r>
+  <r>
+    <n v="1975"/>
+    <x v="0"/>
+    <n v="160.87747035573099"/>
+  </r>
+  <r>
+    <n v="1975"/>
+    <x v="1"/>
+    <m/>
+  </r>
+  <r>
+    <n v="1975"/>
+    <x v="2"/>
+    <m/>
+  </r>
+  <r>
+    <n v="1975"/>
+    <x v="3"/>
+    <n v="4.4256338582677204"/>
+  </r>
+  <r>
+    <n v="1976"/>
+    <x v="0"/>
+    <n v="124.772047244094"/>
+  </r>
+  <r>
+    <n v="1976"/>
+    <x v="1"/>
+    <m/>
+  </r>
+  <r>
+    <n v="1976"/>
+    <x v="2"/>
+    <m/>
+  </r>
+  <r>
+    <n v="1976"/>
+    <x v="3"/>
+    <n v="4.3532274509803903"/>
+  </r>
+  <r>
+    <n v="1977"/>
+    <x v="0"/>
+    <n v="147.792749003984"/>
+  </r>
+  <r>
+    <n v="1977"/>
+    <x v="1"/>
+    <m/>
+  </r>
+  <r>
+    <n v="1977"/>
+    <x v="2"/>
+    <m/>
+  </r>
+  <r>
+    <n v="1977"/>
+    <x v="3"/>
+    <n v="4.6351904761904796"/>
+  </r>
+  <r>
+    <n v="1978"/>
+    <x v="0"/>
+    <n v="193.44365079365099"/>
+  </r>
+  <r>
+    <n v="1978"/>
+    <x v="1"/>
+    <m/>
+  </r>
+  <r>
+    <n v="1978"/>
+    <x v="2"/>
+    <m/>
+  </r>
+  <r>
+    <n v="1978"/>
+    <x v="3"/>
+    <n v="5.42176587301587"/>
+  </r>
+  <r>
+    <n v="1979"/>
+    <x v="0"/>
+    <n v="304.68239999999997"/>
+  </r>
+  <r>
+    <n v="1979"/>
+    <x v="1"/>
+    <m/>
+  </r>
+  <r>
+    <n v="1979"/>
+    <x v="2"/>
+    <m/>
+  </r>
+  <r>
+    <n v="1979"/>
+    <x v="3"/>
+    <n v="11.067905138339899"/>
+  </r>
+  <r>
+    <n v="1980"/>
+    <x v="0"/>
+    <n v="614.49900793650795"/>
+  </r>
+  <r>
+    <n v="1980"/>
+    <x v="1"/>
+    <m/>
+  </r>
+  <r>
+    <n v="1980"/>
+    <x v="2"/>
+    <m/>
+  </r>
+  <r>
+    <n v="1980"/>
+    <x v="3"/>
+    <n v="20.983653543307099"/>
+  </r>
+  <r>
+    <n v="1981"/>
+    <x v="0"/>
+    <n v="459.26004016064297"/>
+  </r>
+  <r>
+    <n v="1981"/>
+    <x v="1"/>
+    <m/>
+  </r>
+  <r>
+    <n v="1981"/>
+    <x v="2"/>
+    <m/>
+  </r>
+  <r>
+    <n v="1981"/>
+    <x v="3"/>
+    <n v="10.486944223107599"/>
+  </r>
+  <r>
+    <n v="1982"/>
+    <x v="0"/>
+    <n v="375.30458167330698"/>
+  </r>
+  <r>
+    <n v="1982"/>
+    <x v="1"/>
+    <m/>
+  </r>
+  <r>
+    <n v="1982"/>
+    <x v="2"/>
+    <m/>
+  </r>
+  <r>
+    <n v="1982"/>
+    <x v="3"/>
+    <n v="7.9218611111111104"/>
+  </r>
+  <r>
+    <n v="1983"/>
+    <x v="0"/>
+    <n v="423.66359999999997"/>
+  </r>
+  <r>
+    <n v="1983"/>
+    <x v="1"/>
+    <m/>
+  </r>
+  <r>
+    <n v="1983"/>
+    <x v="2"/>
+    <m/>
+  </r>
+  <r>
+    <n v="1983"/>
+    <x v="3"/>
+    <n v="11.4147213438735"/>
+  </r>
+  <r>
+    <n v="1984"/>
+    <x v="0"/>
+    <n v="360.78422310757003"/>
+  </r>
+  <r>
+    <n v="1984"/>
+    <x v="1"/>
+    <m/>
+  </r>
+  <r>
+    <n v="1984"/>
+    <x v="2"/>
+    <m/>
+  </r>
+  <r>
+    <n v="1984"/>
+    <x v="3"/>
+    <n v="8.1446031746031693"/>
+  </r>
+  <r>
+    <n v="1985"/>
+    <x v="0"/>
+    <n v="317.29523809523801"/>
+  </r>
+  <r>
+    <n v="1985"/>
+    <x v="1"/>
+    <m/>
+  </r>
+  <r>
+    <n v="1985"/>
+    <x v="2"/>
+    <m/>
+  </r>
+  <r>
+    <n v="1985"/>
+    <x v="3"/>
+    <n v="6.1318715415019804"/>
+  </r>
+  <r>
+    <n v="1986"/>
+    <x v="0"/>
+    <n v="367.85498007968101"/>
+  </r>
+  <r>
+    <n v="1986"/>
+    <x v="1"/>
+    <m/>
+  </r>
+  <r>
+    <n v="1986"/>
+    <x v="2"/>
+    <m/>
+  </r>
+  <r>
+    <n v="1986"/>
+    <x v="3"/>
+    <n v="5.4645197628458497"/>
+  </r>
+  <r>
+    <n v="1987"/>
+    <x v="0"/>
+    <n v="446.223705179283"/>
+  </r>
+  <r>
+    <n v="1987"/>
+    <x v="1"/>
+    <m/>
+  </r>
+  <r>
+    <n v="1987"/>
+    <x v="2"/>
+    <m/>
+  </r>
+  <r>
+    <n v="1987"/>
+    <x v="3"/>
+    <n v="7.0156130952380904"/>
+  </r>
+  <r>
+    <n v="1988"/>
+    <x v="0"/>
+    <n v="436.85816733067702"/>
+  </r>
+  <r>
+    <n v="1988"/>
+    <x v="1"/>
+    <m/>
+  </r>
+  <r>
+    <n v="1988"/>
+    <x v="2"/>
+    <m/>
+  </r>
+  <r>
+    <n v="1988"/>
+    <x v="3"/>
+    <n v="6.5324367588932803"/>
+  </r>
+  <r>
+    <n v="1989"/>
+    <x v="0"/>
+    <n v="380.8202"/>
+  </r>
+  <r>
+    <n v="1989"/>
+    <x v="1"/>
+    <m/>
+  </r>
+  <r>
+    <n v="1989"/>
+    <x v="2"/>
+    <m/>
+  </r>
+  <r>
+    <n v="1989"/>
+    <x v="3"/>
+    <n v="5.4998948412698399"/>
+  </r>
+  <r>
+    <n v="1990"/>
+    <x v="0"/>
+    <n v="383.56454183266902"/>
+  </r>
+  <r>
+    <n v="1990"/>
+    <x v="1"/>
+    <n v="108.751069518717"/>
+  </r>
+  <r>
+    <n v="1990"/>
+    <x v="2"/>
+    <n v="461.27673796791402"/>
+  </r>
+  <r>
+    <n v="1990"/>
+    <x v="3"/>
+    <n v="4.8315889328063202"/>
+  </r>
+  <r>
+    <n v="1991"/>
+    <x v="0"/>
+    <n v="362.25697211155398"/>
+  </r>
+  <r>
+    <n v="1991"/>
+    <x v="1"/>
+    <n v="88.363545816733094"/>
+  </r>
+  <r>
+    <n v="1991"/>
+    <x v="2"/>
+    <n v="376.27151394422299"/>
+  </r>
+  <r>
+    <n v="1991"/>
+    <x v="3"/>
+    <n v="4.0566086956521703"/>
+  </r>
+  <r>
+    <n v="1992"/>
+    <x v="0"/>
+    <n v="343.94920634920601"/>
+  </r>
+  <r>
+    <n v="1992"/>
+    <x v="1"/>
+    <n v="88.134920634920604"/>
+  </r>
+  <r>
+    <n v="1992"/>
+    <x v="2"/>
+    <n v="359.96428571428601"/>
+  </r>
+  <r>
+    <n v="1992"/>
+    <x v="3"/>
+    <n v="3.9464370078740201"/>
+  </r>
+  <r>
+    <n v="1993"/>
+    <x v="0"/>
+    <n v="359.81513944223099"/>
+  </r>
+  <r>
+    <n v="1993"/>
+    <x v="1"/>
+    <n v="122.459362549801"/>
+  </r>
+  <r>
+    <n v="1993"/>
+    <x v="2"/>
+    <n v="373.93725099601602"/>
+  </r>
+  <r>
+    <n v="1993"/>
+    <x v="3"/>
+    <n v="4.3130098814229196"/>
+  </r>
+  <r>
+    <n v="1994"/>
+    <x v="0"/>
+    <n v="384.15140000000002"/>
+  </r>
+  <r>
+    <n v="1994"/>
+    <x v="1"/>
+    <n v="142.7516"/>
+  </r>
+  <r>
+    <n v="1994"/>
+    <x v="2"/>
+    <n v="405.21319999999997"/>
+  </r>
+  <r>
+    <n v="1994"/>
+    <x v="3"/>
+    <n v="5.2851329365079396"/>
+  </r>
+  <r>
+    <n v="1995"/>
+    <x v="0"/>
+    <n v="384.0532"/>
+  </r>
+  <r>
+    <n v="1995"/>
+    <x v="1"/>
+    <n v="151.29"/>
+  </r>
+  <r>
+    <n v="1995"/>
+    <x v="2"/>
+    <n v="424.23540000000003"/>
+  </r>
+  <r>
+    <n v="1995"/>
+    <x v="3"/>
+    <n v="5.1970615079365103"/>
+  </r>
+  <r>
+    <n v="1996"/>
+    <x v="0"/>
+    <n v="387.86785714285702"/>
+  </r>
+  <r>
+    <n v="1996"/>
+    <x v="1"/>
+    <n v="128.121031746032"/>
+  </r>
+  <r>
+    <n v="1996"/>
+    <x v="2"/>
+    <n v="397.42519841269802"/>
+  </r>
+  <r>
+    <n v="1996"/>
+    <x v="3"/>
+    <n v="5.1994527559055097"/>
+  </r>
+  <r>
+    <n v="1997"/>
+    <x v="0"/>
+    <n v="331.29482071713102"/>
+  </r>
+  <r>
+    <n v="1997"/>
+    <x v="1"/>
+    <n v="177.97270916334699"/>
+  </r>
+  <r>
+    <n v="1997"/>
+    <x v="2"/>
+    <n v="395.86494023904402"/>
+  </r>
+  <r>
+    <n v="1997"/>
+    <x v="3"/>
+    <n v="4.8972411067193704"/>
+  </r>
+  <r>
+    <n v="1998"/>
+    <x v="0"/>
+    <n v="294.08705179282902"/>
+  </r>
+  <r>
+    <n v="1998"/>
+    <x v="1"/>
+    <n v="284.123505976096"/>
+  </r>
+  <r>
+    <n v="1998"/>
+    <x v="2"/>
+    <n v="371.77430278884498"/>
+  </r>
+  <r>
+    <n v="1998"/>
+    <x v="3"/>
+    <n v="5.5397944664031602"/>
+  </r>
+  <r>
+    <n v="1999"/>
+    <x v="0"/>
+    <n v="278.57270916334699"/>
+  </r>
+  <r>
+    <n v="1999"/>
+    <x v="1"/>
+    <n v="357.74422310757001"/>
+  </r>
+  <r>
+    <n v="1999"/>
+    <x v="2"/>
+    <n v="376.73187250996"/>
+  </r>
+  <r>
+    <n v="1999"/>
+    <x v="3"/>
+    <n v="5.21840674603175"/>
+  </r>
+  <r>
+    <n v="2000"/>
+    <x v="0"/>
+    <n v="279.10199999999998"/>
+  </r>
+  <r>
+    <n v="2000"/>
+    <x v="1"/>
+    <n v="680.32799999999997"/>
+  </r>
+  <r>
+    <n v="2000"/>
+    <x v="2"/>
+    <n v="544.13800000000003"/>
+  </r>
+  <r>
+    <n v="2000"/>
+    <x v="3"/>
+    <n v="4.9525297619047599"/>
+  </r>
+  <r>
+    <n v="2001"/>
+    <x v="0"/>
+    <n v="271.03585657370502"/>
+  </r>
+  <r>
+    <n v="2001"/>
+    <x v="1"/>
+    <n v="603.68127490039797"/>
+  </r>
+  <r>
+    <n v="2001"/>
+    <x v="2"/>
+    <n v="528.99800796812701"/>
+  </r>
+  <r>
+    <n v="2001"/>
+    <x v="3"/>
+    <n v="4.3702173913043501"/>
+  </r>
+  <r>
+    <n v="2002"/>
+    <x v="0"/>
+    <n v="309.67720000000003"/>
+  </r>
+  <r>
+    <n v="2002"/>
+    <x v="1"/>
+    <n v="337.56"/>
+  </r>
+  <r>
+    <n v="2002"/>
+    <x v="2"/>
+    <n v="539.255"/>
+  </r>
+  <r>
+    <n v="2002"/>
+    <x v="3"/>
+    <n v="4.5990059523809501"/>
+  </r>
+  <r>
+    <n v="2003"/>
+    <x v="0"/>
+    <n v="363.32091633466098"/>
+  </r>
+  <r>
+    <n v="2003"/>
+    <x v="1"/>
+    <n v="200.518924302789"/>
+  </r>
+  <r>
+    <n v="2003"/>
+    <x v="2"/>
+    <n v="691.19322709163396"/>
+  </r>
+  <r>
+    <n v="2003"/>
+    <x v="3"/>
+    <n v="4.8786857707509901"/>
+  </r>
+  <r>
+    <n v="2004"/>
+    <x v="0"/>
+    <n v="409.16626984126998"/>
+  </r>
+  <r>
+    <n v="2004"/>
+    <x v="1"/>
+    <n v="230.22123015873001"/>
+  </r>
+  <r>
+    <n v="2004"/>
+    <x v="2"/>
+    <n v="845.51984126984098"/>
+  </r>
+  <r>
+    <n v="2004"/>
+    <x v="3"/>
+    <n v="6.6578248031496097"/>
+  </r>
+  <r>
+    <n v="2005"/>
+    <x v="0"/>
+    <n v="444.44779999999997"/>
+  </r>
+  <r>
+    <n v="2005"/>
+    <x v="1"/>
+    <n v="201.07900000000001"/>
+  </r>
+  <r>
+    <n v="2005"/>
+    <x v="2"/>
+    <n v="896.57299999999998"/>
+  </r>
+  <r>
+    <n v="2005"/>
+    <x v="3"/>
+    <n v="7.3115376984126996"/>
+  </r>
+  <r>
+    <n v="2006"/>
+    <x v="0"/>
+    <n v="603.7722"/>
+  </r>
+  <r>
+    <n v="2006"/>
+    <x v="1"/>
+    <n v="319.99900000000002"/>
+  </r>
+  <r>
+    <n v="2006"/>
+    <x v="2"/>
+    <n v="1142.5540000000001"/>
+  </r>
+  <r>
+    <n v="2006"/>
+    <x v="3"/>
+    <n v="11.5491765873016"/>
+  </r>
+  <r>
+    <n v="2007"/>
+    <x v="0"/>
+    <n v="695.38645418326701"/>
+  </r>
+  <r>
+    <n v="2007"/>
+    <x v="1"/>
+    <n v="354.77689243027902"/>
+  </r>
+  <r>
+    <n v="2007"/>
+    <x v="2"/>
+    <n v="1302.80677290837"/>
+  </r>
+  <r>
+    <n v="2007"/>
+    <x v="3"/>
+    <n v="13.3835375494071"/>
+  </r>
+  <r>
+    <n v="2008"/>
+    <x v="0"/>
+    <n v="871.96269841269805"/>
+  </r>
+  <r>
+    <n v="2008"/>
+    <x v="1"/>
+    <n v="352.25"/>
+  </r>
+  <r>
+    <n v="2008"/>
+    <x v="2"/>
+    <n v="1577.5337301587299"/>
+  </r>
+  <r>
+    <n v="2008"/>
+    <x v="3"/>
+    <n v="14.989074803149601"/>
+  </r>
+  <r>
+    <n v="2009"/>
+    <x v="0"/>
+    <n v="972.348605577689"/>
+  </r>
+  <r>
+    <n v="2009"/>
+    <x v="1"/>
+    <n v="263.21713147410401"/>
+  </r>
+  <r>
+    <n v="2009"/>
+    <x v="2"/>
+    <n v="1203.5"/>
+  </r>
+  <r>
+    <n v="2009"/>
+    <x v="3"/>
+    <n v="14.6742786561265"/>
+  </r>
+  <r>
+    <n v="2010"/>
+    <x v="0"/>
+    <n v="1224.5209163346599"/>
+  </r>
+  <r>
+    <n v="2010"/>
+    <x v="1"/>
+    <n v="525.24103585657394"/>
+  </r>
+  <r>
+    <n v="2010"/>
+    <x v="2"/>
+    <n v="1608.98406374502"/>
+  </r>
+  <r>
+    <n v="2010"/>
+    <x v="3"/>
+    <n v="20.1928853754941"/>
+  </r>
+  <r>
+    <n v="2011"/>
+    <x v="0"/>
+    <n v="1571.5200803212899"/>
+  </r>
+  <r>
+    <n v="2011"/>
+    <x v="1"/>
+    <n v="733.63453815261005"/>
+  </r>
+  <r>
+    <n v="2011"/>
+    <x v="2"/>
+    <n v="1721.8674698795201"/>
+  </r>
+  <r>
+    <n v="2011"/>
+    <x v="3"/>
+    <n v="35.119203187251003"/>
+  </r>
+  <r>
+    <n v="2012"/>
+    <x v="0"/>
+    <n v="1668.9803999999999"/>
+  </r>
+  <r>
+    <n v="2012"/>
+    <x v="1"/>
+    <n v="643.18799999999999"/>
+  </r>
+  <r>
+    <n v="2012"/>
+    <x v="2"/>
+    <n v="1551.4760000000001"/>
+  </r>
+  <r>
+    <n v="2012"/>
+    <x v="3"/>
+    <n v="31.149682539682502"/>
+  </r>
+  <r>
+    <n v="2013"/>
+    <x v="0"/>
+    <n v="1411.22569721116"/>
+  </r>
+  <r>
+    <n v="2013"/>
+    <x v="1"/>
+    <n v="725.05577689243"/>
+  </r>
+  <r>
+    <n v="2013"/>
+    <x v="2"/>
+    <n v="1486.71912350598"/>
+  </r>
+  <r>
+    <n v="2013"/>
+    <x v="3"/>
+    <n v="23.792786561264801"/>
+  </r>
+  <r>
+    <n v="2014"/>
+    <x v="0"/>
+    <n v="1266.40239043825"/>
+  </r>
+  <r>
+    <n v="2014"/>
+    <x v="1"/>
+    <n v="803.22310756972104"/>
+  </r>
+  <r>
+    <n v="2014"/>
+    <x v="2"/>
+    <n v="1385.7011952191201"/>
+  </r>
+  <r>
+    <n v="2014"/>
+    <x v="3"/>
+    <n v="19.077845849802401"/>
+  </r>
+  <r>
+    <n v="2015"/>
+    <x v="0"/>
+    <n v="1160.06235059761"/>
+  </r>
+  <r>
+    <n v="2015"/>
+    <x v="1"/>
+    <n v="691.62549800796796"/>
+  </r>
+  <r>
+    <n v="2015"/>
+    <x v="2"/>
+    <n v="1053.492"/>
+  </r>
+  <r>
+    <n v="2015"/>
+    <x v="3"/>
+    <n v="15.68"/>
+  </r>
+  <r>
+    <n v="2016"/>
+    <x v="0"/>
+    <n v="1250.7980079681299"/>
+  </r>
+  <r>
+    <n v="2016"/>
+    <x v="1"/>
+    <n v="613.26679841897203"/>
+  </r>
+  <r>
+    <n v="2016"/>
+    <x v="2"/>
+    <n v="988.33464566929104"/>
+  </r>
+  <r>
+    <n v="2016"/>
+    <x v="3"/>
+    <n v="17.137588932806299"/>
+  </r>
+  <r>
+    <n v="2017"/>
+    <x v="0"/>
+    <n v="1257.1454000000001"/>
+  </r>
+  <r>
+    <n v="2017"/>
+    <x v="1"/>
+    <n v="867.45362903225805"/>
+  </r>
+  <r>
+    <n v="2017"/>
+    <x v="2"/>
+    <n v="948.70161290322596"/>
+  </r>
+  <r>
+    <n v="2017"/>
+    <x v="3"/>
+    <n v="17.048055555555599"/>
+  </r>
+  <r>
+    <n v="2018"/>
+    <x v="0"/>
+    <n v="1268.4866533864499"/>
+  </r>
+  <r>
+    <n v="2018"/>
+    <x v="1"/>
+    <n v="1028.3247011952201"/>
+  </r>
+  <r>
+    <n v="2018"/>
+    <x v="2"/>
+    <n v="879.952"/>
+  </r>
+  <r>
+    <n v="2018"/>
+    <x v="3"/>
+    <n v="15.705375494071101"/>
+  </r>
+  <r>
+    <n v="2019"/>
+    <x v="0"/>
+    <n v="1392.5960159362601"/>
+  </r>
+  <r>
+    <n v="2019"/>
+    <x v="1"/>
+    <n v="1533.7991967871501"/>
+  </r>
+  <r>
+    <n v="2019"/>
+    <x v="2"/>
+    <n v="862.20481927710796"/>
+  </r>
+  <r>
+    <n v="2019"/>
+    <x v="3"/>
+    <n v="16.208537549407101"/>
+  </r>
+  <r>
+    <n v="2020"/>
+    <x v="0"/>
+    <n v="1555.03125"/>
+  </r>
+  <r>
+    <n v="2020"/>
+    <x v="1"/>
+    <n v="2212.125"/>
+  </r>
+  <r>
+    <n v="2020"/>
+    <x v="2"/>
+    <n v="988.875"/>
+  </r>
+  <r>
+    <n v="2020"/>
+    <x v="3"/>
+    <n v="18.003125000000001"/>
+  </r>
+</pivotCacheRecords>
+</file>
+
+<file path=xl/pivotTables/pivotTable1.xml><?xml version="1.0" encoding="utf-8"?>
+<pivotTableDefinition xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="xr" xr:uid="{EF9FBE64-E6A6-4278-B011-1D5A72D23B6A}" name="MetalsPivot" cacheId="2" applyNumberFormats="0" applyBorderFormats="0" applyFontFormats="0" applyPatternFormats="0" applyAlignmentFormats="0" applyWidthHeightFormats="1" dataCaption="Values" updatedVersion="8" minRefreshableVersion="3" showCalcMbrs="0" useAutoFormatting="1" itemPrintTitles="1" createdVersion="3" indent="0" outline="1" outlineData="1" multipleFieldFilters="0">
+  <location ref="B4:F10" firstHeaderRow="1" firstDataRow="2" firstDataCol="1"/>
+  <pivotFields count="3">
+    <pivotField showAll="0"/>
+    <pivotField axis="axisRow" showAll="0">
+      <items count="5">
+        <item x="0"/>
+        <item x="1"/>
+        <item x="2"/>
+        <item x="3"/>
+        <item t="default"/>
+      </items>
+    </pivotField>
+    <pivotField dataField="1" showAll="0"/>
+  </pivotFields>
+  <rowFields count="1">
+    <field x="1"/>
+  </rowFields>
+  <rowItems count="5">
+    <i>
+      <x/>
+    </i>
+    <i>
+      <x v="1"/>
+    </i>
+    <i>
+      <x v="2"/>
+    </i>
+    <i>
+      <x v="3"/>
+    </i>
+    <i t="grand">
+      <x/>
+    </i>
+  </rowItems>
+  <colFields count="1">
+    <field x="-2"/>
+  </colFields>
+  <colItems count="4">
+    <i>
+      <x/>
+    </i>
+    <i i="1">
+      <x v="1"/>
+    </i>
+    <i i="2">
+      <x v="2"/>
+    </i>
+    <i i="3">
+      <x v="3"/>
+    </i>
+  </colItems>
+  <dataFields count="4">
+    <dataField name="Min Price" fld="2" subtotal="min" baseField="0" baseItem="0" numFmtId="164"/>
+    <dataField name="Avg Price" fld="2" subtotal="average" baseField="0" baseItem="0" numFmtId="164"/>
+    <dataField name="Max Price" fld="2" subtotal="max" baseField="0" baseItem="0" numFmtId="164"/>
+    <dataField name="Std Price" fld="2" subtotal="stdDev" baseField="0" baseItem="0" numFmtId="164"/>
+  </dataFields>
+  <formats count="43">
+    <format dxfId="42">
+      <pivotArea outline="0" collapsedLevelsAreSubtotals="1" fieldPosition="0">
+        <references count="1">
+          <reference field="4294967294" count="1" selected="0">
+            <x v="0"/>
+          </reference>
+        </references>
+      </pivotArea>
+    </format>
+    <format dxfId="41">
+      <pivotArea field="-2" type="button" dataOnly="0" labelOnly="1" outline="0" axis="axisCol" fieldPosition="0"/>
+    </format>
+    <format dxfId="40">
+      <pivotArea dataOnly="0" labelOnly="1" outline="0" fieldPosition="0">
+        <references count="1">
+          <reference field="4294967294" count="1">
+            <x v="0"/>
+          </reference>
+        </references>
+      </pivotArea>
+    </format>
+    <format dxfId="39">
+      <pivotArea outline="0" collapsedLevelsAreSubtotals="1" fieldPosition="0">
+        <references count="1">
+          <reference field="4294967294" count="1" selected="0">
+            <x v="0"/>
+          </reference>
+        </references>
+      </pivotArea>
+    </format>
+    <format dxfId="38">
+      <pivotArea field="-2" type="button" dataOnly="0" labelOnly="1" outline="0" axis="axisCol" fieldPosition="0"/>
+    </format>
+    <format dxfId="37">
+      <pivotArea dataOnly="0" labelOnly="1" outline="0" fieldPosition="0">
+        <references count="1">
+          <reference field="4294967294" count="1">
+            <x v="0"/>
+          </reference>
+        </references>
+      </pivotArea>
+    </format>
+    <format dxfId="36">
+      <pivotArea outline="0" collapsedLevelsAreSubtotals="1" fieldPosition="0">
+        <references count="1">
+          <reference field="4294967294" count="1" selected="0">
+            <x v="1"/>
+          </reference>
+        </references>
+      </pivotArea>
+    </format>
+    <format dxfId="35">
+      <pivotArea type="topRight" dataOnly="0" labelOnly="1" outline="0" fieldPosition="0"/>
+    </format>
+    <format dxfId="34">
+      <pivotArea dataOnly="0" labelOnly="1" outline="0" fieldPosition="0">
+        <references count="1">
+          <reference field="4294967294" count="1">
+            <x v="1"/>
+          </reference>
+        </references>
+      </pivotArea>
+    </format>
+    <format dxfId="33">
+      <pivotArea outline="0" collapsedLevelsAreSubtotals="1" fieldPosition="0">
+        <references count="1">
+          <reference field="4294967294" count="1" selected="0">
+            <x v="1"/>
+          </reference>
+        </references>
+      </pivotArea>
+    </format>
+    <format dxfId="32">
+      <pivotArea type="topRight" dataOnly="0" labelOnly="1" outline="0" fieldPosition="0"/>
+    </format>
+    <format dxfId="31">
+      <pivotArea dataOnly="0" labelOnly="1" outline="0" fieldPosition="0">
+        <references count="1">
+          <reference field="4294967294" count="1">
+            <x v="1"/>
+          </reference>
+        </references>
+      </pivotArea>
+    </format>
+    <format dxfId="30">
+      <pivotArea outline="0" collapsedLevelsAreSubtotals="1" fieldPosition="0">
+        <references count="1">
+          <reference field="4294967294" count="1" selected="0">
+            <x v="2"/>
+          </reference>
+        </references>
+      </pivotArea>
+    </format>
+    <format dxfId="29">
+      <pivotArea outline="0" collapsedLevelsAreSubtotals="1" fieldPosition="0">
+        <references count="1">
+          <reference field="4294967294" count="1" selected="0">
+            <x v="2"/>
+          </reference>
+        </references>
+      </pivotArea>
+    </format>
+    <format dxfId="28">
+      <pivotArea outline="0" collapsedLevelsAreSubtotals="1" fieldPosition="0">
+        <references count="1">
+          <reference field="4294967294" count="1" selected="0">
+            <x v="3"/>
+          </reference>
+        </references>
+      </pivotArea>
+    </format>
+    <format dxfId="27">
+      <pivotArea outline="0" collapsedLevelsAreSubtotals="1" fieldPosition="0">
+        <references count="1">
+          <reference field="4294967294" count="1" selected="0">
+            <x v="3"/>
+          </reference>
+        </references>
+      </pivotArea>
+    </format>
+    <format dxfId="26">
+      <pivotArea type="all" dataOnly="0" outline="0" fieldPosition="0"/>
+    </format>
+    <format dxfId="25">
+      <pivotArea outline="0" collapsedLevelsAreSubtotals="1" fieldPosition="0"/>
+    </format>
+    <format dxfId="24">
+      <pivotArea type="origin" dataOnly="0" labelOnly="1" outline="0" fieldPosition="0"/>
+    </format>
+    <format dxfId="23">
+      <pivotArea field="-2" type="button" dataOnly="0" labelOnly="1" outline="0" axis="axisCol" fieldPosition="0"/>
+    </format>
+    <format dxfId="22">
+      <pivotArea type="topRight" dataOnly="0" labelOnly="1" outline="0" fieldPosition="0"/>
+    </format>
+    <format dxfId="21">
+      <pivotArea field="1" type="button" dataOnly="0" labelOnly="1" outline="0" axis="axisRow" fieldPosition="0"/>
+    </format>
+    <format dxfId="20">
+      <pivotArea dataOnly="0" labelOnly="1" fieldPosition="0">
+        <references count="1">
+          <reference field="1" count="0"/>
+        </references>
+      </pivotArea>
+    </format>
+    <format dxfId="19">
+      <pivotArea dataOnly="0" labelOnly="1" grandRow="1" outline="0" fieldPosition="0"/>
+    </format>
+    <format dxfId="18">
+      <pivotArea dataOnly="0" labelOnly="1" outline="0" fieldPosition="0">
+        <references count="1">
+          <reference field="4294967294" count="4">
+            <x v="0"/>
+            <x v="1"/>
+            <x v="2"/>
+            <x v="3"/>
+          </reference>
+        </references>
+      </pivotArea>
+    </format>
+    <format dxfId="17">
+      <pivotArea type="all" dataOnly="0" outline="0" fieldPosition="0"/>
+    </format>
+    <format dxfId="16">
+      <pivotArea outline="0" collapsedLevelsAreSubtotals="1" fieldPosition="0"/>
+    </format>
+    <format dxfId="15">
+      <pivotArea type="origin" dataOnly="0" labelOnly="1" outline="0" fieldPosition="0"/>
+    </format>
+    <format dxfId="14">
+      <pivotArea field="-2" type="button" dataOnly="0" labelOnly="1" outline="0" axis="axisCol" fieldPosition="0"/>
+    </format>
+    <format dxfId="13">
+      <pivotArea type="topRight" dataOnly="0" labelOnly="1" outline="0" fieldPosition="0"/>
+    </format>
+    <format dxfId="12">
+      <pivotArea field="1" type="button" dataOnly="0" labelOnly="1" outline="0" axis="axisRow" fieldPosition="0"/>
+    </format>
+    <format dxfId="11">
+      <pivotArea dataOnly="0" labelOnly="1" fieldPosition="0">
+        <references count="1">
+          <reference field="1" count="0"/>
+        </references>
+      </pivotArea>
+    </format>
+    <format dxfId="10">
+      <pivotArea dataOnly="0" labelOnly="1" grandRow="1" outline="0" fieldPosition="0"/>
+    </format>
+    <format dxfId="9">
+      <pivotArea dataOnly="0" labelOnly="1" outline="0" fieldPosition="0">
+        <references count="1">
+          <reference field="4294967294" count="4">
+            <x v="0"/>
+            <x v="1"/>
+            <x v="2"/>
+            <x v="3"/>
+          </reference>
+        </references>
+      </pivotArea>
+    </format>
+    <format dxfId="8">
+      <pivotArea type="all" dataOnly="0" outline="0" fieldPosition="0"/>
+    </format>
+    <format dxfId="7">
+      <pivotArea outline="0" collapsedLevelsAreSubtotals="1" fieldPosition="0"/>
+    </format>
+    <format dxfId="6">
+      <pivotArea type="origin" dataOnly="0" labelOnly="1" outline="0" fieldPosition="0"/>
+    </format>
+    <format dxfId="5">
+      <pivotArea field="-2" type="button" dataOnly="0" labelOnly="1" outline="0" axis="axisCol" fieldPosition="0"/>
+    </format>
+    <format dxfId="4">
+      <pivotArea type="topRight" dataOnly="0" labelOnly="1" outline="0" fieldPosition="0"/>
+    </format>
+    <format dxfId="3">
+      <pivotArea field="1" type="button" dataOnly="0" labelOnly="1" outline="0" axis="axisRow" fieldPosition="0"/>
+    </format>
+    <format dxfId="2">
+      <pivotArea dataOnly="0" labelOnly="1" fieldPosition="0">
+        <references count="1">
+          <reference field="1" count="0"/>
+        </references>
+      </pivotArea>
+    </format>
+    <format dxfId="1">
+      <pivotArea dataOnly="0" labelOnly="1" grandRow="1" outline="0" fieldPosition="0"/>
+    </format>
+    <format dxfId="0">
+      <pivotArea dataOnly="0" labelOnly="1" outline="0" fieldPosition="0">
+        <references count="1">
+          <reference field="4294967294" count="4">
+            <x v="0"/>
+            <x v="1"/>
+            <x v="2"/>
+            <x v="3"/>
+          </reference>
+        </references>
+      </pivotArea>
+    </format>
+  </formats>
+  <pivotTableStyleInfo name="PivotStyleLight16" showRowHeaders="1" showColHeaders="1" showRowStripes="0" showColStripes="0" showLastColumn="1"/>
+  <extLst>
+    <ext xmlns:xpdl="http://schemas.microsoft.com/office/spreadsheetml/2016/pivotdefaultlayout" uri="{747A6164-185A-40DC-8AA5-F01512510D54}">
+      <xpdl:pivotTableDefinition16/>
+    </ext>
+  </extLst>
+</pivotTableDefinition>
 </file>
 
 <file path=xl/theme/theme1.xml><?xml version="1.0" encoding="utf-8"?>
@@ -411,10 +2046,10 @@
 </file>
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{1C291986-E273-4258-83D0-75B8981891C8}">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{A1ED52A3-C8D2-4666-8E8B-F366E88AB614}">
   <dimension ref="A1:C213"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0"/>
+    <sheetView workbookViewId="0"/>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="13.2" x14ac:dyDescent="0.25"/>
   <cols>
@@ -2639,4 +4274,131 @@
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <pageSetup orientation="portrait" r:id="rId1"/>
 </worksheet>
+</file>
+
+<file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{DCAABFB5-EE1B-4AFD-9A33-021165500C3B}">
+  <dimension ref="B4:G10"/>
+  <sheetViews>
+    <sheetView tabSelected="1" workbookViewId="0"/>
+  </sheetViews>
+  <sheetFormatPr defaultRowHeight="13.2" x14ac:dyDescent="0.25"/>
+  <cols>
+    <col min="1" max="1" width="8.88671875" style="1"/>
+    <col min="2" max="2" width="12.5546875" style="1" bestFit="1" customWidth="1"/>
+    <col min="3" max="6" width="12" style="3" bestFit="1" customWidth="1"/>
+    <col min="7" max="7" width="8.88671875" style="3"/>
+    <col min="8" max="16384" width="8.88671875" style="1"/>
+  </cols>
+  <sheetData>
+    <row r="4" spans="2:6" x14ac:dyDescent="0.25">
+      <c r="C4" s="2" t="s">
+        <v>10</v>
+      </c>
+    </row>
+    <row r="5" spans="2:6" x14ac:dyDescent="0.25">
+      <c r="B5" s="4" t="s">
+        <v>7</v>
+      </c>
+      <c r="C5" s="3" t="s">
+        <v>9</v>
+      </c>
+      <c r="D5" s="3" t="s">
+        <v>11</v>
+      </c>
+      <c r="E5" s="3" t="s">
+        <v>12</v>
+      </c>
+      <c r="F5" s="3" t="s">
+        <v>13</v>
+      </c>
+    </row>
+    <row r="6" spans="2:6" x14ac:dyDescent="0.25">
+      <c r="B6" s="5" t="s">
+        <v>3</v>
+      </c>
+      <c r="C6" s="3">
+        <v>35.950236220472398</v>
+      </c>
+      <c r="D6" s="3">
+        <v>553.63836760765685</v>
+      </c>
+      <c r="E6" s="3">
+        <v>1668.9803999999999</v>
+      </c>
+      <c r="F6" s="3">
+        <v>463.12602049140133</v>
+      </c>
+    </row>
+    <row r="7" spans="2:6" x14ac:dyDescent="0.25">
+      <c r="B7" s="5" t="s">
+        <v>4</v>
+      </c>
+      <c r="C7" s="3">
+        <v>88.134920634920604</v>
+      </c>
+      <c r="D7" s="3">
+        <v>502.26711947394904</v>
+      </c>
+      <c r="E7" s="3">
+        <v>2212.125</v>
+      </c>
+      <c r="F7" s="3">
+        <v>459.25976899684053</v>
+      </c>
+    </row>
+    <row r="8" spans="2:6" x14ac:dyDescent="0.25">
+      <c r="B8" s="5" t="s">
+        <v>5</v>
+      </c>
+      <c r="C8" s="3">
+        <v>359.96428571428601</v>
+      </c>
+      <c r="D8" s="3">
+        <v>861.00239394093398</v>
+      </c>
+      <c r="E8" s="3">
+        <v>1721.8674698795201</v>
+      </c>
+      <c r="F8" s="3">
+        <v>445.65076023013847</v>
+      </c>
+    </row>
+    <row r="9" spans="2:6" x14ac:dyDescent="0.25">
+      <c r="B9" s="5" t="s">
+        <v>6</v>
+      </c>
+      <c r="C9" s="3">
+        <v>1.53633333333333</v>
+      </c>
+      <c r="D9" s="3">
+        <v>9.4462370035938115</v>
+      </c>
+      <c r="E9" s="3">
+        <v>35.119203187251003</v>
+      </c>
+      <c r="F9" s="3">
+        <v>7.4787431193807841</v>
+      </c>
+    </row>
+    <row r="10" spans="2:6" x14ac:dyDescent="0.25">
+      <c r="B10" s="5" t="s">
+        <v>8</v>
+      </c>
+      <c r="C10" s="3">
+        <v>1.53633333333333</v>
+      </c>
+      <c r="D10" s="3">
+        <v>429.19547000153347</v>
+      </c>
+      <c r="E10" s="3">
+        <v>2212.125</v>
+      </c>
+      <c r="F10" s="3">
+        <v>486.62583686560862</v>
+      </c>
+    </row>
+  </sheetData>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+</worksheet>
 </file>
</xml_diff>